<commit_message>
working on verilog comments. Asm code is done.
</commit_message>
<xml_diff>
--- a/RegisterMappings.xlsx
+++ b/RegisterMappings.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab29b3b8207ead18/Documents/School/PSU/ECE540-DesignOfSoC/Assignments/Project1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive\Documents\School\PSU\ECE540-DesignOfSoC\Assignments\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{74D2DFD7-C12E-4E99-AABA-43B08F68C4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE0C01CA-554E-460A-83AF-656AAB7703E3}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{74D2DFD7-C12E-4E99-AABA-43B08F68C4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93E756FE-319C-48E3-8881-D6DF4D593654}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A848E089-1BB7-4AD6-AA91-27EC376CAC57}"/>
+    <workbookView xWindow="-5910" yWindow="10515" windowWidth="12045" windowHeight="13410" xr2:uid="{A848E089-1BB7-4AD6-AA91-27EC376CAC57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,9 +141,6 @@
     <t>Seven Seg Lower (3:0) Digits value address</t>
   </si>
   <si>
-    <t>Seven Seg Upper (7:4) Digits value address</t>
-  </si>
-  <si>
     <t>Seven Seg Decimal Point enable address</t>
   </si>
   <si>
@@ -167,6 +163,9 @@
   </si>
   <si>
     <t>BusBlaster Clock 476khz</t>
+  </si>
+  <si>
+    <t>Decimal Point Value register</t>
   </si>
 </sst>
 </file>
@@ -211,13 +210,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,9 +615,9 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1029 4218 15328,'6'23'276,"2"-1"1,0 0 0,2-1-1,1 2-276,-7-18 321,-1-1 0,2 1 0,-1-1 0,0 0 0,1 0 0,-1-1 0,1 1 0,0-1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,3 0-321,-8-1 9,1-1 0,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 0,-1-1 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1-1 1,-1 0-1,1 1 0,-1-2-9,9-50-15,-8 45 38,5-45-19,-1 23-6,-2-2 1,-1 1-1,-1 0 1,-3-15 1,1 36-1,1-1 1,0 1 0,0 0 0,1 0-1,1-9 1,5-32-16,-5 38-2,7 3-10,0-1-28,-8 11 54,1-1-1,-1 1 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0 1 1,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 0 2,5 5-14,3 2 7,-1-1 1,0 1 0,0 0-1,-1 0 1,0 1-1,0 0 1,-1 0 0,0 0-1,1 4 7,22 28-28,-25-39 20,3-2 2,-4-1 6,0 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,-1-1 1,2-2 0,1-2 0,4-4 0,0-1 0,0 0 0,-1 0 0,-1 0 0,0-1 0,0 0 0,-2 0 0,1 0 0,0-7 0,-2 11 0,0 0 0,-1-1 0,1 1 0,-1-1 0,-1 0 0,0 0 0,0-2 0,0 0 0,0 1 0,0 0 0,1 0 0,0-1 0,1-1 0,4-27 11,-6 38 12,27 11 55,-14-1-67,2 0 25,1 1 0,0-2 0,0 0 1,1-1-1,8 3-36,-23-9 4,1 0 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,-1-1-1,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 0,-1-1 1,1 1-1,0-1 1,-1 1-1,0-1 1,1 1-1,-1-2-4,7-20 168,-1 1-3097,2 1-11044</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7452.123">41 1757 14616,'4'3'265,"9"11"31,-6-7-182,-1 1 1,-1 0-1,0 1 1,0-1-1,0 1 1,-1 0-1,-1 0 1,1 1-1,-2-1 1,1 1-1,-1-1 1,0 1-1,-1 0 1,0 9-115,9 41 421,-3-31-322,-2-12-21,-1 0 0,0 0 0,-1 1-1,-1-1 1,-1 1 0,0-1 0,-2 11-78,1-21 32,0 0 1,0-1-1,1 1 1,0-1-1,0 1 1,0-1 0,1 1-1,0-1 1,0 0-1,1 0 1,0 0-1,1 2-32,0 0 69,-1 0 1,0 1-1,0-1 0,0 1 0,-1 0 0,1 6-69,-4 111 600,1-127-589,0 1 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1-11,-54-141 256,27 24-151,13 55-49,3 0 0,2-7-56,7 60 9,0 0 0,0 0 0,-1 0-1,0 1 1,-3-6-9,2 6 7,1-1 0,0 1 0,0-1 0,1 1 0,0-7-7,-9-19 25,9 30-20,1 1-1,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0-3-4,2-20 24,-2 24-21,0-1 1,0 1 0,0-1 0,1 1 0,-1-1-1,1 1 1,0 0 0,0-1 0,1-1-4,4-24 50,-7 27-48,1 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,0 1-1,1-1 0,-1 1 1,1-1-1,-1 0 1,1 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0 0-1,1 0 0,-1-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-2,12-6 4,-10 4-3,1 0-1,-1 1 1,1-1 0,0 1-1,0 0 1,0 0 0,0 1-1,0 0 1,0-1 0,0 2 0,0-1-1,1 1 1,-1-1 0,0 2-1,4-1 0,4 3 0,-8-2 0,-1-1 0,1 1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 3 0,-3-3 0,36 55 1,-35-53 1,-1 0-1,0 0 0,-1 0 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,-1 1 0,0-1 0,0 1 1,-1 3-2,0 11 5,1-16-4,0 0 0,0 0 1,0 0-1,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 3-1,-25 46 19,22-40-14,0 1 0,-1-1 0,0 0 0,-1-1 0,-1 0 0,1 0 0,-2 0 0,-7 7-5,-67 68 20,81-82-14,7-4-5,10-6-2,20-22 1,-28 21-1,1 1 1,0 1-1,0 0 1,1 0-1,0 0 1,0 1 0,0 1-1,0-1 1,1 1-1,-1 1 1,1 0-1,0 0 1,0 1-1,1 0 1,-1 1-1,3 0 1,0 3-10,-11-2 8,-1 0 1,0 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,0 1-1,1 0 1,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,-1 2 1,2 0-4,4 6 0,-1 1 0,0 0 0,0 0 1,-1 1-1,0-1 0,-1 1 0,0 0 0,0 0 0,-1 0 0,-1 0 1,0 0-1,-1 0 0,0 0 0,0 1 0,-1-1 0,-1 0 0,0 0 1,0 0-1,-3 6 4,-8 5-1,0 0 1,-2-1-1,-1 0 1,9-12 0,5-6 14,-1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,-3 0-14,5 1-90,-1-1-1,1 0 0,-1 0 1,0-1-1,1 1 0,-1 0 0,0-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0-1 91,-4-10-12559</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7452.125">41 1757 14616,'4'3'265,"9"11"31,-6-7-182,-1 1 1,-1 0-1,0 1 1,0-1-1,0 1 1,-1 0-1,-1 0 1,1 1-1,-2-1 1,1 1-1,-1-1 1,0 1-1,-1 0 1,0 9-115,9 41 421,-3-31-322,-2-12-21,-1 0 0,0 0 0,-1 1-1,-1-1 1,-1 1 0,0-1 0,-2 11-78,1-21 32,0 0 1,0-1-1,1 1 1,0-1-1,0 1 1,0-1 0,1 1-1,0-1 1,0 0-1,1 0 1,0 0-1,1 2-32,0 0 69,-1 0 1,0 1-1,0-1 0,0 1 0,-1 0 0,1 6-69,-4 111 600,1-127-589,0 1 0,-1-1 1,1 1-1,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1-11,-54-141 256,27 24-151,13 55-49,3 0 0,2-7-56,7 60 9,0 0 0,0 0 0,-1 0-1,0 1 1,-3-6-9,2 6 7,1-1 0,0 1 0,0-1 0,1 1 0,0-7-7,-9-19 25,9 30-20,1 1-1,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0-3-4,2-20 24,-2 24-21,0-1 1,0 1 0,0-1 0,1 1 0,-1-1-1,1 1 1,0 0 0,0-1 0,1-1-4,4-24 50,-7 27-48,1 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,0 1-1,1-1 0,-1 1 1,1-1-1,-1 0 1,1 1-1,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,0 1 1,0 0-1,1 0 0,-1-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-2,12-6 4,-10 4-3,1 0-1,-1 1 1,1-1 0,0 1-1,0 0 1,0 0 0,0 1-1,0 0 1,0-1 0,0 2 0,0-1-1,1 1 1,-1-1 0,0 2-1,4-1 0,4 3 0,-8-2 0,-1-1 0,1 1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 3 0,-3-3 0,36 55 1,-35-53 1,-1 0-1,0 0 0,-1 0 0,1 1 1,-1-1-1,0 1 0,0-1 0,0 1 1,0-1-1,-1 1 0,0-1 0,0 1 1,-1 3-2,0 11 5,1-16-4,0 0 0,0 0 1,0 0-1,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 3-1,-25 46 19,22-40-14,0 1 0,-1-1 0,0 0 0,-1-1 0,-1 0 0,1 0 0,-2 0 0,-7 7-5,-67 68 20,81-82-14,7-4-5,10-6-2,20-22 1,-28 21-1,1 1 1,0 1-1,0 0 1,1 0-1,0 0 1,0 1 0,0 1-1,0-1 1,1 1-1,-1 1 1,1 0-1,0 0 1,0 1-1,1 0 1,-1 1-1,3 0 1,0 3-10,-11-2 8,-1 0 1,0 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,0 1-1,1 0 1,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 0 0,-1 2 1,2 0-4,4 6 0,-1 1 0,0 0 0,0 0 1,-1 1-1,0-1 0,-1 1 0,0 0 0,0 0 0,-1 0 0,-1 0 1,0 0-1,-1 0 0,0 0 0,0 1 0,-1-1 0,-1 0 0,0 0 1,0 0-1,-3 6 4,-8 5-1,0 0 1,-2-1-1,-1 0 1,9-12 0,5-6 14,-1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,-3 0-14,5 1-90,-1-1-1,1 0 0,-1 0 1,0-1-1,1 1 0,-1 0 0,0-1 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,0-1 91,-4-10-12559</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-6897.167">410 1939 13896,'3'-1'70,"1"0"0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0-70,9 2 210,4-1 129,-1 2 0,0 0 0,15 7-339,-25-9 61,0 0 0,-1 1-1,1 0 1,-1 0 0,0 1 0,0-1-1,0 1 1,0 0 0,-1 0 0,0 1-1,3 2-60,27 45 450,15 18 114,-47-67-446,0 2-6,3 7 28,-3-6 145,1-21-152,3-29-2,-2 1 0,-2-1 0,-2 0 0,-4-24-131,-7 30 108,8 31-26,0-1-1,0-1 0,1 1 0,0 0 0,0-8-81,2 15 100,-10-12 250,2-5-2650,8 10-9933</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-6532.124">858 1616 15064,'0'0'-2,"1"8"264,-1 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,-2-1 1,1 1-1,-1 0 1,0-1 0,-1 0-1,0 1 1,0-1-1,-1 0 1,0 0-263,1-3 63,2-3-29,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1-1,1 0-33,-1 0 18,-1-1-1,1 1 1,0-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,0 0-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,0 0 1,1 1-1,-1-1 1,1 0-1,-1 0-17,97-7 131,-91 7-116,1 1 0,-1 0 0,0 0 0,0 0 0,1 1-1,-1 1 1,0-1 0,0 1 0,1 1-15,-7-3 2,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0 0,0 1-1,1-1 1,-1 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1-1,-10 14 7,0 0 0,-1-1 0,-1-1-1,0 0 1,0 0 0,-10 5-7,-22 22 29,36-33-7,2 1 4,-3-5 4,8-3-23,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-7,-5-6-2540,0-2-9999</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-6532.126">858 1616 15064,'0'0'-2,"1"8"264,-1 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,-2-1 1,1 1-1,-1 0 1,0-1 0,-1 0-1,0 1 1,0-1-1,-1 0 1,0 0-263,1-3 63,2-3-29,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1-1,1 0-33,-1 0 18,-1-1-1,1 1 1,0-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,0 0-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,0-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,0 0 1,1 1-1,-1-1 1,1 0-1,-1 0-17,97-7 131,-91 7-116,1 1 0,-1 0 0,0 0 0,0 0 0,1 1-1,-1 1 1,0-1 0,0 1 0,1 1-15,-7-3 2,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,-1-1 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 0 0,0 1-1,1-1 1,-1 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0 1-1,0-1-1,-10 14 7,0 0 0,-1-1 0,-1-1-1,0 0 1,0 0 0,-10 5-7,-22 22 29,36-33-7,2 1 4,-3-5 4,8-3-23,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-7,-5-6-2540,0-2-9999</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-5434.303">1202 1271 13896,'46'116'2205,"-32"-82"-1599,-1 0 1,-1 1 0,-2 1-607,19 39 325,-22-60-281,-1 1 0,0 0 0,-1-1 0,-1 1 0,0 1 0,0 4-44,-3-7 23,-1-4-3,1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,1-1 0,3 6-19,-5-14 60,-1 34 640,-26-72-437,-22-48-84,13 20-118,-35-72-14,61 121-45,0-1 0,2 0 1,-5-14-3,-10-22-1,18 44-11,1 0 0,-1 0 0,2 0-1,-1 0 1,1-1 0,1 1-1,-1-1 1,2 0 0,-1-5 12,3 7-34,-1 5 26,1 0-1,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,3-2 9,9-10-20,-12 11 17,1 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,1 0 1,0 1-1,-1 0 0,1-1 0,0 1 1,0 1-1,0-1 0,0 0 3,2 0-5,1 0 0,-2-1 1,1 0-1,0 0 0,0-1 0,5-2 5,12-8-26,0 2 1,1 0-1,0 2 0,4 0 26,18 16 7,-44-6-5,-1 0-1,1 1 1,0-1-1,-1 1 1,1-1-1,-1 1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 1 1,1-1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,0 0-2,-6 12 6,-1-1 0,-1 0-1,0-1 1,-9 9-6,16-18 1,-49 79 7,45-74-12,-1 1-1,2-1 0,-1 1 0,2 1 0,-1-1 0,1 1 0,0 0 1,1 0-1,0 0 0,1 1 0,-1 4 5,4-15-1,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 1 0,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,1 1 0,-1-1-1,0 0 1,1 0-1,-1 1 1,0-1 0,1 0-1,-1 0 1,0 0 0,1 1-1,-1-1 1,1 0 0,-1 0-1,0 0 1,1 0 1,20-2-18,36-19 25,-20 6-8,-10 8 4,-18 4-3,1 0 0,-1 0 1,1 1-1,0 1 0,0-1 1,0 2-1,0-1 0,0 1 0,0 1 1,0 0-1,-1 0 0,5 2 0,8 1 4,9 4-32,-30-8 27,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 1,-2 12-15,0 1 0,-1-1 0,0 0 0,-1 0 0,-1-1 1,0 1-1,-1-1 0,0 0 0,-1 0 0,0-1 0,-1 0 0,0 0 1,0-1-1,-8 7 15,-22 11-127,31-24 114,0 1 0,0-1 1,1 1-1,0 0 0,0 1 0,0 1 13,2-2-8,-26 14-5,29-19 12,-8 0-2303,1-1-9215</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-5082.647">1700 1033 15776,'12'14'200,"-1"0"0,-1 0 0,0 1 0,-1 0 1,0 1-1,-2 0 0,0 0 0,0 1 0,-2 0 1,0 0-1,-1 1 0,1 8-200,-3-12 273,1 0-1,0-1 0,1 1 1,5 11-273,-6-20 12,-1 0 1,0 1 0,0 0 0,-1 0 0,0-1-1,0 1 1,0 0 0,-1 5-13,19 138 564,-19-147-452,0-2 17,0 0-6,0 0-20,0 0-3,0-2-142,-1 0 1,1 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,0-1 41,0-6-1791,2-23-10735</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-4643.357">2127 1025 10848,'0'2'45,"-1"-1"0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 1,1 0-1,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-45,-32 35 1481,25-26-1115,-9 12 211,13-17-363,1 1-1,-1-1 0,0 1 0,0-1 1,0-1-1,-1 1 0,0-1 1,-4 3-214,8-5 93,-1 1 0,1-1 0,0 1 0,0 0 0,1-1 0,-1 1 1,0 0-1,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,1 1-1,-1 2-93,-10 29 700,11-32-653,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,1-1 1,0 1-1,0 0 1,-1 0-1,1-1 1,0 1-1,0-1 1,1 0-1,-1 0 1,2 2-48,-2-3 13,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,-1-1 0,1 1 0,0-1-13,8-7 50,17-12 63,-23 19-105,0 1 1,-1-1-1,1 0 1,0 0-1,-1-1 0,1 1 1,-1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 0,-1-1 1,1 1-1,-1 0 1,1-3-9,1-26 84,-1 27-74,0-1 1,0 1-1,-1 0 0,0 0 1,0 0-1,0-1 1,-1 1-1,0 0 1,0 0-1,0 0 0,-1 0-10,-35-111 144,37 115-139,1 0-2,-1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0-2,-6 1 30,3 13-25,3 11-8,2-16 4,0 1 0,0 0 0,1 0 0,0-1 0,1 1 0,0-1 0,0 0 0,1 0 0,0 0-1,24 51-1,-26-47 1,7 12 0,31 16 0,-6-11 18,-32-28-10,2-1 6,-3-1 2,-1-3-69,0 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,-1 0-1,1 0 1,0 1-1,-1-1 1,0 0-1,0-1 54,-1-6-1850,-4-20-10769</inkml:trace>
@@ -657,7 +658,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1610 10848,'0'0'17,"0"0"4,0 0-2,0 0 46,0 0 173,18 12 1051,-15-2-1082,0 0 1,-1 1-1,-1 0 0,1 0 0,-1-1 1,-1 1-1,0 0 0,-1 4-207,1-3 131,0 1 74,0 0 0,1 1 0,1-1 0,0 0 1,1 0-206,-1 0 386,-2-11-342,-1 0 0,2 0-1,-1 1 1,0-1 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,1 1-1,0-1 1,-1 0 0,1 1 0,0-1-44,0-1 27,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,0 1 0,1-1 1,-1 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,1-1-27,4-4 105,7-2-30,1-1 30,1 0-1,-2-1 1,0-1-1,0 0 1,-1 0 0,0-2-1,7-10-104,-17 21 47,0 0-1,0-1 1,1 1-1,-1 0 1,1 1-1,0-1 1,0 1-1,2-1-46,12-9 129,-5 5 39,-13 7-160,1 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,-1-1 0,0 1 1,1 0-1,-1-1 0,0 1 0,1 0 1,-1-1-1,0 1 0,0-1 1,1 1-1,-1 0 0,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,-1 1 1,1-1-1,0 1-8,3-3 138,0 0-171,-11-6 505,4 6-451,-1 0 0,1 1 0,0-1 0,-1 1 0,0 0-1,0 0 1,1 0 0,-4 0-21,-23-6-2400,28 8-9710</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="357.925">202 1486 12824,'4'4'159,"-2"-3"49,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 1-208,3 8 340,1-1 0,1-1 0,-1 1-1,2-1 1,4 6-340,22 27 794,-29-34-719,0-2-26,-1 1 1,1 0-1,-1 0 0,0 1 1,-1-1-1,0 1 0,0 0 1,-1 0-1,0 0 0,1 3-49,-4-8 22,2-1-1,-1 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,1 1-22,2 7 30,-1 3 25,0 0 0,1-1 0,1 1 0,0-1-1,1 2-54,11 27 136,-17-39-54,1 6 2,3-2-4,-4-44 142,1 18-181,-2 16-328,1 0 0,-1-1 0,0 1 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-3-3 287,4 7-7,-13-23-11879</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="357.924">202 1486 12824,'4'4'159,"-2"-3"49,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 1-208,3 8 340,1-1 0,1-1 0,-1 1-1,2-1 1,4 6-340,22 27 794,-29-34-719,0-2-26,-1 1 1,1 0-1,-1 0 0,0 1 1,-1-1-1,0 1 0,0 0 1,-1 0-1,0 0 0,1 3-49,-4-8 22,2-1-1,-1 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,1 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,1 1-22,2 7 30,-1 3 25,0 0 0,1-1 0,1 1 0,0-1-1,1 2-54,11 27 136,-17-39-54,1 6 2,3-2-4,-4-44 142,1 18-181,-2 16-328,1 0 0,-1-1 0,0 1 0,-1 0-1,1 0 1,-1 1 0,1-1 0,-3-3 287,4 7-7,-13-23-11879</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="748.697">396 1381 9592,'6'22'1974,"2"-27"1042,8-12-2686,1-9 95,-3 0 0,0-1 0,-1-1 0,2-10-425,-12 32 67,3-17 119,-5 20-145,0 0 1,0 0-1,-1 0 0,2 0 0,-1 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1-41,1-1 43,12-18 140,-13 16-129,-2 4-49,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,1 0 0,-1 1 0,0-1 1,1 0-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 0 0,1 1 1,0-1-1,-1 1 0,1-1 1,-1 1-1,1 0 0,0-1 0,0 1 1,-1 0-1,1-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 1 1,1-1-1,0 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 0,1-1 1,-1 1-1,1 0-5,22 38 17,-17-22-4,0 1 0,-1 1 0,-2-1 0,1 0 0,-2 6-13,5 20 26,16 140 235,-22-183-253,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,0 1-8,17 12 141,-17-13-132,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 1 0,0-1-1,1 0 1,0 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 1-1,-1-1 1,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1-1-1,-1 1 1,1 0-1,0 0 1,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,1 1 0,-1-1-1,0 0 1,0 1-1,1-1 1,-1 1 0,0-1-1,0 0-9,5-29 80,-7 12-2405,0 1-9341</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1109.798">520 1469 14344,'8'-1'173,"1"0"0,-1 0 0,0-1 0,0 0 0,0-1 0,0 1 0,-1-2 0,1 1 0,-1-1 1,0 0-1,3-3-173,2-1 284,0 0 0,0-1 0,-1-1 0,-1 0-1,1-1 1,-1 0-284,21-42 928,-8 9-2989,-22 42-9485</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1519.138">786 1027 12640,'1'3'69,"-1"-2"-30,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1 0-1,1 0 0,0-1 1,-1 1-1,1 0 1,-1 0-40,-4 6 985,5-5-750,-1 1 0,1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,1-1-235,1 11 404,-3-5-295,0 0 1,1 0-1,0 0 1,1 0-1,0-1 1,0 1-1,1 0 1,-1 0-1,2-1 1,-1 1-1,1-1 1,0 0-1,2 2-109,2 2 74,0-1 0,1-1-1,1 1 1,-1-1 0,1-1 0,1 0 0,-1 0-1,1-1 1,1 0 0,8 4-74,-18-10 3,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0-3,4-2 5,0 1 0,0-1-1,0-1 1,-1 1-1,0-1 1,0 0 0,0 0-1,0 0-4,11-14 22,-1 0 0,-1-2-1,5-9-21,-16 26 6,19-42 41,-21 43-42,1 0 0,-1-1-1,1 1 1,-1 0 0,0-1-1,1 1 1,-1 0 0,-1-1-1,1 1 1,0-1 0,0 1-1,-1 0 1,0 0-1,1-1 1,-1 1 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-2-2-4,1 3 42,2 1 3,0 0-43,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 1,0 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1-2,-4 3 9,0-1 0,0 1 0,0 0-1,0 1 1,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,0 1 0,0 0-9,-9 9 24,10-12-18,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 3-6,-6 15 24,5-14-10,1-1 1,0 0 0,1 1 0,-1 0 0,1-1 0,0 1-1,0 0 1,1 0 0,-1 4-15,2-2 35,2 0-2,4 0-18,-7-8-44,1 1 1,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,0 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,-1 0-1,1 0 1,0-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,1-1 0,-1 0 28,1 0-1333,9-5-11200</inkml:trace>
@@ -968,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEB8F5C-88E0-440E-BEF4-346E35862D34}">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H21:H22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,9 +1160,6 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1182,7 +1180,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,7 +1191,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,7 +1202,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,7 +1213,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,6 +1234,9 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1322,10 +1323,10 @@
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37">
         <v>476190</v>
@@ -1333,7 +1334,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D38">
         <f>D37/5</f>
@@ -1354,7 +1355,78 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="D39">
+        <f>D37/10</f>
+        <v>47619</v>
+      </c>
+      <c r="E39">
+        <f>$D$39*E36</f>
+        <v>95238</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39:M39" si="0">$D$39*F36</f>
+        <v>142857</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>190476</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>238095</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>285714</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>333333</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>380952</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>428571</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>476190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C43" s="4">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C44" s="5">
+        <f>C42/C43</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F44">
+        <f>1/C44</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>